<commit_message>
备用时间 21:00 -> 21:45
</commit_message>
<xml_diff>
--- a/doc/C10038019.xlsx
+++ b/doc/C10038019.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="8300" yWindow="460" windowWidth="25600" windowHeight="14440"/>
+    <workbookView xWindow="-20" yWindow="460" windowWidth="25600" windowHeight="14440"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1266,7 +1266,7 @@
       <charset val="134"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1288,6 +1288,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1354,7 +1360,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1389,6 +1395,15 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="20" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1749,8 +1764,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N750"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I57" workbookViewId="0">
-      <selection activeCell="I41" sqref="A41:XFD41"/>
+    <sheetView tabSelected="1" topLeftCell="C66" workbookViewId="0">
+      <selection activeCell="N85" sqref="N85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4351,33 +4366,33 @@
         <v>42482.670833333337</v>
       </c>
     </row>
-    <row r="77" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="7">
+    <row r="77" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A77" s="12">
         <v>174773642</v>
       </c>
-      <c r="B77" s="7">
+      <c r="B77" s="12">
         <v>1461359400</v>
       </c>
-      <c r="C77" s="7">
+      <c r="C77" s="12">
         <v>1461368400</v>
       </c>
-      <c r="D77" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="E77" s="8" t="s">
+      <c r="D77" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="E77" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="F77" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="G77" s="8" t="s">
+      <c r="F77" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="G77" s="13" t="s">
         <v>140</v>
       </c>
-      <c r="I77" s="9">
+      <c r="I77" s="14">
         <f t="shared" si="4"/>
         <v>42482.881944444445</v>
       </c>
-      <c r="J77" s="9">
+      <c r="J77" s="14">
         <f t="shared" si="5"/>
         <v>42482.986111111109</v>
       </c>

</xml_diff>